<commit_message>
add spellbook base EN.xml edit spellbook base EN.xlsx
</commit_message>
<xml_diff>
--- a/src/Spellbooks/spellbook base EN.xlsx
+++ b/src/Spellbooks/spellbook base EN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magieny\AndroidStudioProjects\DND5-Spellbook\src\Spellbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A962C59B-51DD-46A6-A5F0-DFF851BC5419}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0947AF29-8CFC-4FDE-B909-8189235F8CDA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{BE30A2F2-96E2-4A1C-829F-2B9479891854}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4606" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4612" uniqueCount="1284">
   <si>
     <t>Level</t>
   </si>
@@ -4253,8 +4253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36C391A-D982-45C9-8F26-E4C83DD2D220}">
   <dimension ref="A1:AJ362"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="R337" sqref="R337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4263,6 +4263,11 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" customWidth="1"/>
     <col min="30" max="32" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4447,7 +4452,9 @@
         <v>37</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="R3" s="3" t="s">
         <v>38</v>
       </c>
@@ -5705,7 +5712,9 @@
         <v>42</v>
       </c>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="R23" s="3" t="s">
         <v>133</v>
       </c>
@@ -9703,7 +9712,9 @@
         <v>26</v>
       </c>
       <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
+      <c r="Q86" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="R86" s="3" t="s">
         <v>240</v>
       </c>
@@ -20613,7 +20624,9 @@
         <v>26</v>
       </c>
       <c r="P258" s="1"/>
-      <c r="Q258" s="1"/>
+      <c r="Q258" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="R258" s="3" t="s">
         <v>958</v>
       </c>
@@ -20787,7 +20800,9 @@
         <v>26</v>
       </c>
       <c r="P261" s="1"/>
-      <c r="Q261" s="1"/>
+      <c r="Q261" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="R261" s="3" t="s">
         <v>355</v>
       </c>
@@ -21789,7 +21804,9 @@
         <v>49</v>
       </c>
       <c r="P277" s="1"/>
-      <c r="Q277" s="1"/>
+      <c r="Q277" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="R277" s="3" t="s">
         <v>1012</v>
       </c>

</xml_diff>